<commit_message>
RPA-121 : Start lesing av kommune nummer
</commit_message>
<xml_diff>
--- a/Vasklister/Excel/vaskeliste_Mai2017.xlsx
+++ b/Vasklister/Excel/vaskeliste_Mai2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="28380" windowHeight="15210"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="27825" windowHeight="15210"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>debitor_ident</t>
   </si>
   <si>
     <t>Sak_Nr</t>
+  </si>
+  <si>
+    <t>Kommune_Nr</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,29 +392,42 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
+        <v>13098245418</v>
+      </c>
+      <c r="B2" s="1">
+        <v>313054</v>
+      </c>
+      <c r="C2">
+        <v>11111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>13088334935</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>267794</v>
       </c>
+      <c r="C3">
+        <v>22222</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>13098245418</v>
-      </c>
-      <c r="B3" s="1">
-        <v>313054</v>
-      </c>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>